<commit_message>
Cleaned up Cor_Analyis R script - ready for revision 2 submission
</commit_message>
<xml_diff>
--- a/Correlation_Analysis/Cor_Base.xlsx
+++ b/Correlation_Analysis/Cor_Base.xlsx
@@ -87,38 +87,57 @@
     <t>6</t>
   </si>
   <si>
-    <t>crop_fertiliserN_uptake</t>
-  </si>
-  <si>
-    <t>crop_soilN_uptake</t>
-  </si>
-  <si>
     <t>yield_Mgha</t>
   </si>
   <si>
-    <t xml:space="preserve">soil_fertiliserN_recovery </t>
-  </si>
-  <si>
     <t>Total phenols</t>
   </si>
   <si>
-    <t>Cinnamic_phenols</t>
-  </si>
-  <si>
-    <t>Syringyl_phenols</t>
-  </si>
-  <si>
-    <t>Vanillyl_phenols</t>
-  </si>
-  <si>
-    <t>p-hydroxybenzoic_phenols</t>
+    <t>p-hydroxybenzoic phenols</t>
+  </si>
+  <si>
+    <t>Vanillyl phenols</t>
+  </si>
+  <si>
+    <t>Cinnamic phenols</t>
+  </si>
+  <si>
+    <t>Syringyl phenols</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soil FertilizerN Recovery </t>
+  </si>
+  <si>
+    <r>
+      <t>Crop N uptake (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fertilizer)</t>
+    </r>
+  </si>
+  <si>
+    <t>Crop N uptake (soil)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,9 +166,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,16 +452,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:M1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.88671875" customWidth="1"/>
+    <col min="10" max="10" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -459,31 +483,31 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>20</v>
-      </c>
-      <c r="K1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -1036,7 +1060,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:M1"/>
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1051,12 +1075,12 @@
     <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.5546875" customWidth="1"/>
-    <col min="11" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1070,31 +1094,31 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>20</v>
-      </c>
-      <c r="K1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>